<commit_message>
added tdms read at once
</commit_message>
<xml_diff>
--- a/data/DAQ-sim.xlsx
+++ b/data/DAQ-sim.xlsx
@@ -3934,7 +3934,7 @@
     </row>
     <row r="209" spans="1:5">
       <c r="A209" s="2">
-        <v>44158.65325328211</v>
+        <v>44158.65325328213</v>
       </c>
       <c r="B209">
         <v>2.07</v>
@@ -3968,7 +3968,7 @@
     </row>
     <row r="211" spans="1:5">
       <c r="A211" s="2">
-        <v>44158.6532535136</v>
+        <v>44158.65325351361</v>
       </c>
       <c r="B211">
         <v>2.09</v>
@@ -4002,7 +4002,7 @@
     </row>
     <row r="213" spans="1:5">
       <c r="A213" s="2">
-        <v>44158.65325374508</v>
+        <v>44158.65325374509</v>
       </c>
       <c r="B213">
         <v>2.11</v>
@@ -7385,7 +7385,7 @@
     </row>
     <row r="412" spans="1:5">
       <c r="A412" s="2">
-        <v>44158.65327677749</v>
+        <v>44158.6532767775</v>
       </c>
       <c r="B412">
         <v>4.1</v>
@@ -7453,7 +7453,7 @@
     </row>
     <row r="416" spans="1:5">
       <c r="A416" s="2">
-        <v>44158.65327724045</v>
+        <v>44158.65327724046</v>
       </c>
       <c r="B416">
         <v>4.14</v>
@@ -7589,7 +7589,7 @@
     </row>
     <row r="424" spans="1:5">
       <c r="A424" s="2">
-        <v>44158.65327816638</v>
+        <v>44158.65327816639</v>
       </c>
       <c r="B424">
         <v>4.22</v>
@@ -14066,7 +14066,7 @@
     </row>
     <row r="805" spans="1:5">
       <c r="A805" s="2">
-        <v>44158.6533222636</v>
+        <v>44158.65332226361</v>
       </c>
       <c r="B805">
         <v>8.029999999999999</v>
@@ -14202,7 +14202,7 @@
     </row>
     <row r="813" spans="1:5">
       <c r="A813" s="2">
-        <v>44158.65332318952</v>
+        <v>44158.65332318954</v>
       </c>
       <c r="B813">
         <v>8.109999999999999</v>
@@ -14338,7 +14338,7 @@
     </row>
     <row r="821" spans="1:5">
       <c r="A821" s="2">
-        <v>44158.65332411545</v>
+        <v>44158.65332411546</v>
       </c>
       <c r="B821">
         <v>8.19</v>
@@ -14355,7 +14355,7 @@
     </row>
     <row r="822" spans="1:5">
       <c r="A822" s="2">
-        <v>44158.65332423119</v>
+        <v>44158.65332423121</v>
       </c>
       <c r="B822">
         <v>8.199999999999999</v>
@@ -14491,7 +14491,7 @@
     </row>
     <row r="830" spans="1:5">
       <c r="A830" s="2">
-        <v>44158.65332515712</v>
+        <v>44158.65332515713</v>
       </c>
       <c r="B830">
         <v>8.279999999999999</v>
@@ -14763,7 +14763,7 @@
     </row>
     <row r="846" spans="1:5">
       <c r="A846" s="2">
-        <v>44158.65332700897</v>
+        <v>44158.65332700898</v>
       </c>
       <c r="B846">
         <v>8.44</v>
@@ -14780,7 +14780,7 @@
     </row>
     <row r="847" spans="1:5">
       <c r="A847" s="2">
-        <v>44158.65332712471</v>
+        <v>44158.65332712472</v>
       </c>
       <c r="B847">
         <v>8.449999999999999</v>
@@ -14916,7 +14916,7 @@
     </row>
     <row r="855" spans="1:5">
       <c r="A855" s="2">
-        <v>44158.65332805063</v>
+        <v>44158.65332805065</v>
       </c>
       <c r="B855">
         <v>8.529999999999999</v>
@@ -27717,7 +27717,7 @@
     </row>
     <row r="1608" spans="1:5">
       <c r="A1608" s="2">
-        <v>44158.65341520341</v>
+        <v>44158.65341520343</v>
       </c>
       <c r="B1608">
         <v>16.06</v>
@@ -27836,7 +27836,7 @@
     </row>
     <row r="1615" spans="1:5">
       <c r="A1615" s="2">
-        <v>44158.6534160136</v>
+        <v>44158.65341601361</v>
       </c>
       <c r="B1615">
         <v>16.13</v>
@@ -27870,7 +27870,7 @@
     </row>
     <row r="1617" spans="1:5">
       <c r="A1617" s="2">
-        <v>44158.65341624508</v>
+        <v>44158.65341624509</v>
       </c>
       <c r="B1617">
         <v>16.15</v>
@@ -27989,7 +27989,7 @@
     </row>
     <row r="1624" spans="1:5">
       <c r="A1624" s="2">
-        <v>44158.65341705527</v>
+        <v>44158.65341705528</v>
       </c>
       <c r="B1624">
         <v>16.22</v>
@@ -28142,7 +28142,7 @@
     </row>
     <row r="1633" spans="1:5">
       <c r="A1633" s="2">
-        <v>44158.65341809693</v>
+        <v>44158.65341809695</v>
       </c>
       <c r="B1633">
         <v>16.31</v>
@@ -28261,7 +28261,7 @@
     </row>
     <row r="1640" spans="1:5">
       <c r="A1640" s="2">
-        <v>44158.65341890712</v>
+        <v>44158.65341890713</v>
       </c>
       <c r="B1640">
         <v>16.38</v>
@@ -28295,7 +28295,7 @@
     </row>
     <row r="1642" spans="1:5">
       <c r="A1642" s="2">
-        <v>44158.6534191386</v>
+        <v>44158.65341913861</v>
       </c>
       <c r="B1642">
         <v>16.4</v>
@@ -28567,7 +28567,7 @@
     </row>
     <row r="1658" spans="1:5">
       <c r="A1658" s="2">
-        <v>44158.65342099045</v>
+        <v>44158.65342099046</v>
       </c>
       <c r="B1658">
         <v>16.56</v>
@@ -28686,7 +28686,7 @@
     </row>
     <row r="1665" spans="1:5">
       <c r="A1665" s="2">
-        <v>44158.65342180063</v>
+        <v>44158.65342180065</v>
       </c>
       <c r="B1665">
         <v>16.63</v>
@@ -28720,7 +28720,7 @@
     </row>
     <row r="1667" spans="1:5">
       <c r="A1667" s="2">
-        <v>44158.65342203212</v>
+        <v>44158.65342203213</v>
       </c>
       <c r="B1667">
         <v>16.65</v>
@@ -28839,7 +28839,7 @@
     </row>
     <row r="1674" spans="1:5">
       <c r="A1674" s="2">
-        <v>44158.6534228423</v>
+        <v>44158.65342284231</v>
       </c>
       <c r="B1674">
         <v>16.72</v>
@@ -28992,7 +28992,7 @@
     </row>
     <row r="1683" spans="1:5">
       <c r="A1683" s="2">
-        <v>44158.65342388397</v>
+        <v>44158.65342388398</v>
       </c>
       <c r="B1683">
         <v>16.81</v>
@@ -29111,7 +29111,7 @@
     </row>
     <row r="1690" spans="1:5">
       <c r="A1690" s="2">
-        <v>44158.65342469415</v>
+        <v>44158.65342469417</v>
       </c>
       <c r="B1690">
         <v>16.88</v>
@@ -29145,7 +29145,7 @@
     </row>
     <row r="1692" spans="1:5">
       <c r="A1692" s="2">
-        <v>44158.65342492564</v>
+        <v>44158.65342492565</v>
       </c>
       <c r="B1692">
         <v>16.9</v>
@@ -29264,7 +29264,7 @@
     </row>
     <row r="1699" spans="1:5">
       <c r="A1699" s="2">
-        <v>44158.65342573582</v>
+        <v>44158.65342573584</v>
       </c>
       <c r="B1699">
         <v>16.97</v>
@@ -29417,7 +29417,7 @@
     </row>
     <row r="1708" spans="1:5">
       <c r="A1708" s="2">
-        <v>44158.65342677749</v>
+        <v>44158.6534267775</v>
       </c>
       <c r="B1708">
         <v>17.06</v>
@@ -54832,7 +54832,7 @@
     </row>
     <row r="3203" spans="1:5">
       <c r="A3203" s="2">
-        <v>44158.6535998099</v>
+        <v>44158.65359980991</v>
       </c>
       <c r="B3203">
         <v>32.01</v>
@@ -54900,7 +54900,7 @@
     </row>
     <row r="3207" spans="1:5">
       <c r="A3207" s="2">
-        <v>44158.65360027286</v>
+        <v>44158.65360027287</v>
       </c>
       <c r="B3207">
         <v>32.05</v>
@@ -55138,7 +55138,7 @@
     </row>
     <row r="3221" spans="1:5">
       <c r="A3221" s="2">
-        <v>44158.65360189323</v>
+        <v>44158.65360189324</v>
       </c>
       <c r="B3221">
         <v>32.19</v>
@@ -55325,7 +55325,7 @@
     </row>
     <row r="3232" spans="1:5">
       <c r="A3232" s="2">
-        <v>44158.65360316638</v>
+        <v>44158.65360316639</v>
       </c>
       <c r="B3232">
         <v>32.3</v>
@@ -55444,7 +55444,7 @@
     </row>
     <row r="3239" spans="1:5">
       <c r="A3239" s="2">
-        <v>44158.65360397656</v>
+        <v>44158.65360397657</v>
       </c>
       <c r="B3239">
         <v>32.37</v>

</xml_diff>